<commit_message>
Add intra-session tests (group)
</commit_message>
<xml_diff>
--- a/AOAnova/RW_Reciprocity_Repeatability_Analysis_.xlsx
+++ b/AOAnova/RW_Reciprocity_Repeatability_Analysis_.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dhb/Documents/MATLAB/projects/Analysis/AdaptiveOpticsAnalysis/AOAnova/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B85AB1A-9DEA-304F-A910-C343BE38CAF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B224BE0-A2F9-2D44-A89E-829133AA65C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-37620" yWindow="0" windowWidth="32480" windowHeight="21600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13360" yWindow="5040" windowWidth="32480" windowHeight="21600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Reciprocity Statistics" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="39">
   <si>
     <t>153nW</t>
   </si>
@@ -146,6 +146,12 @@
   </si>
   <si>
     <t>Stimulus</t>
+  </si>
+  <si>
+    <t>Resp</t>
+  </si>
+  <si>
+    <t>Group</t>
   </si>
 </sst>
 </file>
@@ -2211,10 +2217,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A2:Z23"/>
+  <dimension ref="A2:Z43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N15" sqref="N15"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2248,10 +2254,10 @@
         <v>34</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="O3" s="7" t="s">
         <v>35</v>
@@ -2260,10 +2266,10 @@
         <v>34</v>
       </c>
       <c r="Q3" s="7" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="R3" s="7" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -2273,11 +2279,11 @@
       <c r="B4" s="5">
         <v>1</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4" s="5">
         <v>4.5551000000000004</v>
-      </c>
-      <c r="D4" s="5">
-        <v>3.984</v>
       </c>
       <c r="F4" t="s">
         <v>5</v>
@@ -2288,11 +2294,11 @@
       <c r="P4" s="5">
         <v>1</v>
       </c>
-      <c r="Q4" s="5">
+      <c r="Q4">
+        <v>1</v>
+      </c>
+      <c r="R4" s="5">
         <v>4.1835000000000004</v>
-      </c>
-      <c r="R4" s="5">
-        <v>4.5785</v>
       </c>
       <c r="T4" t="s">
         <v>5</v>
@@ -2305,11 +2311,11 @@
       <c r="B5" s="5">
         <v>2</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5" s="5">
         <v>4.5209999999999999</v>
-      </c>
-      <c r="D5" s="5">
-        <v>4.2622999999999998</v>
       </c>
       <c r="F5" s="4" t="s">
         <v>30</v>
@@ -2332,11 +2338,11 @@
       <c r="P5" s="5">
         <v>2</v>
       </c>
-      <c r="Q5" s="5">
+      <c r="Q5">
+        <v>1</v>
+      </c>
+      <c r="R5" s="5">
         <v>4.1134000000000004</v>
-      </c>
-      <c r="R5" s="5">
-        <v>4.5646000000000004</v>
       </c>
       <c r="T5" s="4" t="s">
         <v>30</v>
@@ -2361,11 +2367,11 @@
       <c r="B6" s="5">
         <v>3</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6" s="5">
         <v>4.8205</v>
-      </c>
-      <c r="D6" s="5">
-        <v>4.6292999999999997</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>27</v>
@@ -2388,11 +2394,11 @@
       <c r="P6" s="5">
         <v>3</v>
       </c>
-      <c r="Q6" s="5">
+      <c r="Q6">
+        <v>1</v>
+      </c>
+      <c r="R6" s="5">
         <v>4.1486000000000001</v>
-      </c>
-      <c r="R6" s="5">
-        <v>4.1680999999999999</v>
       </c>
       <c r="T6" s="1" t="s">
         <v>27</v>
@@ -2417,11 +2423,11 @@
       <c r="B7" s="5">
         <v>4</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7" s="5">
         <v>4.9162999999999997</v>
-      </c>
-      <c r="D7" s="5">
-        <v>4.9283000000000001</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>28</v>
@@ -2444,11 +2450,11 @@
       <c r="P7" s="5">
         <v>4</v>
       </c>
-      <c r="Q7" s="5">
+      <c r="Q7">
+        <v>1</v>
+      </c>
+      <c r="R7" s="5">
         <v>3.1766000000000001</v>
-      </c>
-      <c r="R7" s="5">
-        <v>4.0476999999999999</v>
       </c>
       <c r="T7" s="3" t="s">
         <v>28</v>
@@ -2473,11 +2479,11 @@
       <c r="B8" s="5">
         <v>5</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8" s="5">
         <v>4.8445</v>
-      </c>
-      <c r="D8" s="5">
-        <v>5.0427999999999997</v>
       </c>
       <c r="O8" s="5">
         <v>11002</v>
@@ -2485,11 +2491,11 @@
       <c r="P8" s="5">
         <v>5</v>
       </c>
-      <c r="Q8" s="5">
+      <c r="Q8">
+        <v>1</v>
+      </c>
+      <c r="R8" s="5">
         <v>4.1554000000000002</v>
-      </c>
-      <c r="R8" s="5">
-        <v>4.0164</v>
       </c>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.2">
@@ -2499,11 +2505,11 @@
       <c r="B9" s="5">
         <v>1</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9" s="5">
         <v>2.1589</v>
-      </c>
-      <c r="D9" s="5">
-        <v>2.972</v>
       </c>
       <c r="O9" s="5">
         <v>11057</v>
@@ -2511,11 +2517,11 @@
       <c r="P9" s="5">
         <v>1</v>
       </c>
-      <c r="Q9" s="5">
+      <c r="Q9">
+        <v>1</v>
+      </c>
+      <c r="R9" s="5">
         <v>3.3216000000000001</v>
-      </c>
-      <c r="R9" s="5">
-        <v>3.5661999999999998</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -2525,11 +2531,11 @@
       <c r="B10" s="5">
         <v>2</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10" s="5">
         <v>2.6341000000000001</v>
-      </c>
-      <c r="D10" s="5">
-        <v>2.3220000000000001</v>
       </c>
       <c r="F10" t="s">
         <v>11</v>
@@ -2540,11 +2546,11 @@
       <c r="P10" s="5">
         <v>2</v>
       </c>
-      <c r="Q10" s="5">
+      <c r="Q10">
+        <v>1</v>
+      </c>
+      <c r="R10" s="5">
         <v>3.3795999999999999</v>
-      </c>
-      <c r="R10" s="5">
-        <v>3.59</v>
       </c>
       <c r="T10" t="s">
         <v>11</v>
@@ -2557,11 +2563,11 @@
       <c r="B11" s="5">
         <v>3</v>
       </c>
-      <c r="C11" s="5">
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11" s="5">
         <v>2.5419999999999998</v>
-      </c>
-      <c r="D11" s="5">
-        <v>2.7309000000000001</v>
       </c>
       <c r="F11" s="4" t="s">
         <v>12</v>
@@ -2590,11 +2596,11 @@
       <c r="P11" s="5">
         <v>3</v>
       </c>
-      <c r="Q11" s="5">
+      <c r="Q11">
+        <v>1</v>
+      </c>
+      <c r="R11" s="5">
         <v>3.302</v>
-      </c>
-      <c r="R11" s="5">
-        <v>3.1556999999999999</v>
       </c>
       <c r="T11" s="4" t="s">
         <v>12</v>
@@ -2625,11 +2631,11 @@
       <c r="B12" s="5">
         <v>4</v>
       </c>
-      <c r="C12" s="5">
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12" s="5">
         <v>2.9980000000000002</v>
-      </c>
-      <c r="D12" s="5">
-        <v>2.8187000000000002</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>31</v>
@@ -2658,11 +2664,11 @@
       <c r="P12" s="5">
         <v>4</v>
       </c>
-      <c r="Q12" s="5">
+      <c r="Q12">
+        <v>1</v>
+      </c>
+      <c r="R12" s="5">
         <v>3.4218000000000002</v>
-      </c>
-      <c r="R12" s="5">
-        <v>3.1133999999999999</v>
       </c>
       <c r="T12" s="1" t="s">
         <v>31</v>
@@ -2693,11 +2699,11 @@
       <c r="B13" s="5">
         <v>5</v>
       </c>
-      <c r="C13" s="5">
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13" s="5">
         <v>2.8119999999999998</v>
-      </c>
-      <c r="D13" s="5">
-        <v>2.9215</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>32</v>
@@ -2720,11 +2726,11 @@
       <c r="P13" s="5">
         <v>5</v>
       </c>
-      <c r="Q13" s="5">
+      <c r="Q13">
+        <v>1</v>
+      </c>
+      <c r="R13" s="5">
         <v>3.605</v>
-      </c>
-      <c r="R13" s="5">
-        <v>3.58</v>
       </c>
       <c r="T13" s="1" t="s">
         <v>32</v>
@@ -2749,11 +2755,11 @@
       <c r="B14" s="5">
         <v>1</v>
       </c>
-      <c r="C14" s="5">
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14" s="5">
         <v>2.8096999999999999</v>
-      </c>
-      <c r="D14" s="5">
-        <v>2.7021000000000002</v>
       </c>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
@@ -2768,11 +2774,11 @@
       <c r="P14" s="5">
         <v>1</v>
       </c>
-      <c r="Q14" s="5">
+      <c r="Q14">
+        <v>1</v>
+      </c>
+      <c r="R14" s="5">
         <v>3.2883</v>
-      </c>
-      <c r="R14" s="5">
-        <v>2.911</v>
       </c>
       <c r="T14" s="1"/>
       <c r="U14" s="1"/>
@@ -2789,11 +2795,11 @@
       <c r="B15" s="5">
         <v>2</v>
       </c>
-      <c r="C15" s="5">
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15" s="5">
         <v>3.1785000000000001</v>
-      </c>
-      <c r="D15" s="5">
-        <v>3.2</v>
       </c>
       <c r="F15" s="3" t="s">
         <v>6</v>
@@ -2814,11 +2820,11 @@
       <c r="P15" s="5">
         <v>2</v>
       </c>
-      <c r="Q15" s="5">
+      <c r="Q15">
+        <v>1</v>
+      </c>
+      <c r="R15" s="5">
         <v>3.2995000000000001</v>
-      </c>
-      <c r="R15" s="5">
-        <v>2.8378999999999999</v>
       </c>
       <c r="T15" s="3" t="s">
         <v>6</v>
@@ -2841,11 +2847,11 @@
       <c r="B16" s="5">
         <v>3</v>
       </c>
-      <c r="C16" s="5">
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16" s="5">
         <v>3.4561000000000002</v>
-      </c>
-      <c r="D16" s="5">
-        <v>3.2254999999999998</v>
       </c>
       <c r="O16" s="5">
         <v>11108</v>
@@ -2853,11 +2859,11 @@
       <c r="P16" s="5">
         <v>3</v>
       </c>
-      <c r="Q16" s="5">
+      <c r="Q16">
+        <v>1</v>
+      </c>
+      <c r="R16" s="5">
         <v>3.2530000000000001</v>
-      </c>
-      <c r="R16" s="5">
-        <v>3.1657000000000002</v>
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.2">
@@ -2867,11 +2873,11 @@
       <c r="B17" s="5">
         <v>4</v>
       </c>
-      <c r="C17" s="5">
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17" s="5">
         <v>3.7456</v>
-      </c>
-      <c r="D17" s="5">
-        <v>2.9350000000000001</v>
       </c>
       <c r="O17" s="5">
         <v>11108</v>
@@ -2879,11 +2885,11 @@
       <c r="P17" s="5">
         <v>4</v>
       </c>
-      <c r="Q17" s="5">
+      <c r="Q17">
+        <v>1</v>
+      </c>
+      <c r="R17" s="5">
         <v>3.1150000000000002</v>
-      </c>
-      <c r="R17" s="5">
-        <v>3.3003</v>
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.2">
@@ -2893,11 +2899,11 @@
       <c r="B18" s="5">
         <v>5</v>
       </c>
-      <c r="C18" s="5">
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18" s="5">
         <v>2.6009000000000002</v>
-      </c>
-      <c r="D18" s="5">
-        <v>3.1173999999999999</v>
       </c>
       <c r="O18" s="5">
         <v>11108</v>
@@ -2905,11 +2911,11 @@
       <c r="P18" s="5">
         <v>5</v>
       </c>
-      <c r="Q18" s="5">
+      <c r="Q18">
+        <v>1</v>
+      </c>
+      <c r="R18" s="5">
         <v>3.1488999999999998</v>
-      </c>
-      <c r="R18" s="5">
-        <v>3.7035</v>
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.2">
@@ -2919,11 +2925,11 @@
       <c r="B19" s="5">
         <v>1</v>
       </c>
-      <c r="C19" s="5">
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19" s="5">
         <v>1.6719999999999999</v>
-      </c>
-      <c r="D19" s="5">
-        <v>2.3041</v>
       </c>
       <c r="O19" s="5">
         <v>11112</v>
@@ -2931,11 +2937,11 @@
       <c r="P19" s="5">
         <v>1</v>
       </c>
-      <c r="Q19" s="5">
+      <c r="Q19">
+        <v>1</v>
+      </c>
+      <c r="R19" s="5">
         <v>2.6928000000000001</v>
-      </c>
-      <c r="R19" s="5">
-        <v>2.7675999999999998</v>
       </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.2">
@@ -2945,11 +2951,11 @@
       <c r="B20" s="5">
         <v>2</v>
       </c>
-      <c r="C20" s="5">
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20" s="5">
         <v>2.2176999999999998</v>
-      </c>
-      <c r="D20" s="5">
-        <v>2.0830000000000002</v>
       </c>
       <c r="O20" s="5">
         <v>11112</v>
@@ -2957,11 +2963,11 @@
       <c r="P20" s="5">
         <v>2</v>
       </c>
-      <c r="Q20" s="5">
+      <c r="Q20">
+        <v>1</v>
+      </c>
+      <c r="R20" s="5">
         <v>3.0409000000000002</v>
-      </c>
-      <c r="R20" s="5">
-        <v>2.2237</v>
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.2">
@@ -2971,11 +2977,11 @@
       <c r="B21" s="5">
         <v>3</v>
       </c>
-      <c r="C21" s="5">
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21" s="5">
         <v>2.4321000000000002</v>
-      </c>
-      <c r="D21" s="5">
-        <v>2.3456999999999999</v>
       </c>
       <c r="O21" s="5">
         <v>11112</v>
@@ -2983,11 +2989,11 @@
       <c r="P21" s="5">
         <v>3</v>
       </c>
-      <c r="Q21" s="5">
+      <c r="Q21">
+        <v>1</v>
+      </c>
+      <c r="R21" s="5">
         <v>2.5383</v>
-      </c>
-      <c r="R21" s="5">
-        <v>2.6067999999999998</v>
       </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.2">
@@ -2997,11 +3003,11 @@
       <c r="B22" s="5">
         <v>4</v>
       </c>
-      <c r="C22" s="5">
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22" s="5">
         <v>2.7351000000000001</v>
-      </c>
-      <c r="D22" s="5">
-        <v>2.6530999999999998</v>
       </c>
       <c r="O22" s="5">
         <v>11112</v>
@@ -3009,11 +3015,11 @@
       <c r="P22" s="5">
         <v>4</v>
       </c>
-      <c r="Q22" s="5">
+      <c r="Q22">
+        <v>1</v>
+      </c>
+      <c r="R22" s="5">
         <v>2.5951</v>
-      </c>
-      <c r="R22" s="5">
-        <v>3.1389999999999998</v>
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.2">
@@ -3023,11 +3029,11 @@
       <c r="B23" s="5">
         <v>5</v>
       </c>
-      <c r="C23" s="5">
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23" s="5">
         <v>2.1021000000000001</v>
-      </c>
-      <c r="D23" s="5">
-        <v>2.9794999999999998</v>
       </c>
       <c r="O23" s="5">
         <v>11112</v>
@@ -3035,10 +3041,530 @@
       <c r="P23" s="5">
         <v>5</v>
       </c>
-      <c r="Q23" s="5">
+      <c r="Q23">
+        <v>1</v>
+      </c>
+      <c r="R23" s="5">
         <v>2.6928000000000001</v>
       </c>
-      <c r="R23" s="5">
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A24" s="5">
+        <v>11002</v>
+      </c>
+      <c r="B24" s="5">
+        <v>1</v>
+      </c>
+      <c r="C24">
+        <v>2</v>
+      </c>
+      <c r="D24" s="5">
+        <v>3.984</v>
+      </c>
+      <c r="O24" s="5">
+        <v>11002</v>
+      </c>
+      <c r="P24" s="5">
+        <v>1</v>
+      </c>
+      <c r="Q24">
+        <v>2</v>
+      </c>
+      <c r="R24" s="5">
+        <v>4.5785</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A25" s="5">
+        <v>11002</v>
+      </c>
+      <c r="B25" s="5">
+        <v>2</v>
+      </c>
+      <c r="C25">
+        <v>2</v>
+      </c>
+      <c r="D25" s="5">
+        <v>4.2622999999999998</v>
+      </c>
+      <c r="O25" s="5">
+        <v>11002</v>
+      </c>
+      <c r="P25" s="5">
+        <v>2</v>
+      </c>
+      <c r="Q25">
+        <v>2</v>
+      </c>
+      <c r="R25" s="5">
+        <v>4.5646000000000004</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A26" s="5">
+        <v>11002</v>
+      </c>
+      <c r="B26" s="5">
+        <v>3</v>
+      </c>
+      <c r="C26">
+        <v>2</v>
+      </c>
+      <c r="D26" s="5">
+        <v>4.6292999999999997</v>
+      </c>
+      <c r="O26" s="5">
+        <v>11002</v>
+      </c>
+      <c r="P26" s="5">
+        <v>3</v>
+      </c>
+      <c r="Q26">
+        <v>2</v>
+      </c>
+      <c r="R26" s="5">
+        <v>4.1680999999999999</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A27" s="5">
+        <v>11002</v>
+      </c>
+      <c r="B27" s="5">
+        <v>4</v>
+      </c>
+      <c r="C27">
+        <v>2</v>
+      </c>
+      <c r="D27" s="5">
+        <v>4.9283000000000001</v>
+      </c>
+      <c r="O27" s="5">
+        <v>11002</v>
+      </c>
+      <c r="P27" s="5">
+        <v>4</v>
+      </c>
+      <c r="Q27">
+        <v>2</v>
+      </c>
+      <c r="R27" s="5">
+        <v>4.0476999999999999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A28" s="5">
+        <v>11002</v>
+      </c>
+      <c r="B28" s="5">
+        <v>5</v>
+      </c>
+      <c r="C28">
+        <v>2</v>
+      </c>
+      <c r="D28" s="5">
+        <v>5.0427999999999997</v>
+      </c>
+      <c r="O28" s="5">
+        <v>11002</v>
+      </c>
+      <c r="P28" s="5">
+        <v>5</v>
+      </c>
+      <c r="Q28">
+        <v>2</v>
+      </c>
+      <c r="R28" s="5">
+        <v>4.0164</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A29" s="5">
+        <v>11057</v>
+      </c>
+      <c r="B29" s="5">
+        <v>1</v>
+      </c>
+      <c r="C29">
+        <v>2</v>
+      </c>
+      <c r="D29" s="5">
+        <v>2.972</v>
+      </c>
+      <c r="O29" s="5">
+        <v>11057</v>
+      </c>
+      <c r="P29" s="5">
+        <v>1</v>
+      </c>
+      <c r="Q29">
+        <v>2</v>
+      </c>
+      <c r="R29" s="5">
+        <v>3.5661999999999998</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A30" s="5">
+        <v>11057</v>
+      </c>
+      <c r="B30" s="5">
+        <v>2</v>
+      </c>
+      <c r="C30">
+        <v>2</v>
+      </c>
+      <c r="D30" s="5">
+        <v>2.3220000000000001</v>
+      </c>
+      <c r="O30" s="5">
+        <v>11057</v>
+      </c>
+      <c r="P30" s="5">
+        <v>2</v>
+      </c>
+      <c r="Q30">
+        <v>2</v>
+      </c>
+      <c r="R30" s="5">
+        <v>3.59</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A31" s="5">
+        <v>11057</v>
+      </c>
+      <c r="B31" s="5">
+        <v>3</v>
+      </c>
+      <c r="C31">
+        <v>2</v>
+      </c>
+      <c r="D31" s="5">
+        <v>2.7309000000000001</v>
+      </c>
+      <c r="O31" s="5">
+        <v>11057</v>
+      </c>
+      <c r="P31" s="5">
+        <v>3</v>
+      </c>
+      <c r="Q31">
+        <v>2</v>
+      </c>
+      <c r="R31" s="5">
+        <v>3.1556999999999999</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A32" s="5">
+        <v>11057</v>
+      </c>
+      <c r="B32" s="5">
+        <v>4</v>
+      </c>
+      <c r="C32">
+        <v>2</v>
+      </c>
+      <c r="D32" s="5">
+        <v>2.8187000000000002</v>
+      </c>
+      <c r="O32" s="5">
+        <v>11057</v>
+      </c>
+      <c r="P32" s="5">
+        <v>4</v>
+      </c>
+      <c r="Q32">
+        <v>2</v>
+      </c>
+      <c r="R32" s="5">
+        <v>3.1133999999999999</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A33" s="5">
+        <v>11057</v>
+      </c>
+      <c r="B33" s="5">
+        <v>5</v>
+      </c>
+      <c r="C33">
+        <v>2</v>
+      </c>
+      <c r="D33" s="5">
+        <v>2.9215</v>
+      </c>
+      <c r="O33" s="5">
+        <v>11057</v>
+      </c>
+      <c r="P33" s="5">
+        <v>5</v>
+      </c>
+      <c r="Q33">
+        <v>2</v>
+      </c>
+      <c r="R33" s="5">
+        <v>3.58</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A34" s="5">
+        <v>11108</v>
+      </c>
+      <c r="B34" s="5">
+        <v>1</v>
+      </c>
+      <c r="C34">
+        <v>2</v>
+      </c>
+      <c r="D34" s="5">
+        <v>2.7021000000000002</v>
+      </c>
+      <c r="O34" s="5">
+        <v>11108</v>
+      </c>
+      <c r="P34" s="5">
+        <v>1</v>
+      </c>
+      <c r="Q34">
+        <v>2</v>
+      </c>
+      <c r="R34" s="5">
+        <v>2.911</v>
+      </c>
+    </row>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A35" s="5">
+        <v>11108</v>
+      </c>
+      <c r="B35" s="5">
+        <v>2</v>
+      </c>
+      <c r="C35">
+        <v>2</v>
+      </c>
+      <c r="D35" s="5">
+        <v>3.2</v>
+      </c>
+      <c r="O35" s="5">
+        <v>11108</v>
+      </c>
+      <c r="P35" s="5">
+        <v>2</v>
+      </c>
+      <c r="Q35">
+        <v>2</v>
+      </c>
+      <c r="R35" s="5">
+        <v>2.8378999999999999</v>
+      </c>
+    </row>
+    <row r="36" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A36" s="5">
+        <v>11108</v>
+      </c>
+      <c r="B36" s="5">
+        <v>3</v>
+      </c>
+      <c r="C36">
+        <v>2</v>
+      </c>
+      <c r="D36" s="5">
+        <v>3.2254999999999998</v>
+      </c>
+      <c r="O36" s="5">
+        <v>11108</v>
+      </c>
+      <c r="P36" s="5">
+        <v>3</v>
+      </c>
+      <c r="Q36">
+        <v>2</v>
+      </c>
+      <c r="R36" s="5">
+        <v>3.1657000000000002</v>
+      </c>
+    </row>
+    <row r="37" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A37" s="5">
+        <v>11108</v>
+      </c>
+      <c r="B37" s="5">
+        <v>4</v>
+      </c>
+      <c r="C37">
+        <v>2</v>
+      </c>
+      <c r="D37" s="5">
+        <v>2.9350000000000001</v>
+      </c>
+      <c r="O37" s="5">
+        <v>11108</v>
+      </c>
+      <c r="P37" s="5">
+        <v>4</v>
+      </c>
+      <c r="Q37">
+        <v>2</v>
+      </c>
+      <c r="R37" s="5">
+        <v>3.3003</v>
+      </c>
+    </row>
+    <row r="38" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A38" s="5">
+        <v>11108</v>
+      </c>
+      <c r="B38" s="5">
+        <v>5</v>
+      </c>
+      <c r="C38">
+        <v>2</v>
+      </c>
+      <c r="D38" s="5">
+        <v>3.1173999999999999</v>
+      </c>
+      <c r="O38" s="5">
+        <v>11108</v>
+      </c>
+      <c r="P38" s="5">
+        <v>5</v>
+      </c>
+      <c r="Q38">
+        <v>2</v>
+      </c>
+      <c r="R38" s="5">
+        <v>3.7035</v>
+      </c>
+    </row>
+    <row r="39" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A39" s="5">
+        <v>11112</v>
+      </c>
+      <c r="B39" s="5">
+        <v>1</v>
+      </c>
+      <c r="C39">
+        <v>2</v>
+      </c>
+      <c r="D39" s="5">
+        <v>2.3041</v>
+      </c>
+      <c r="O39" s="5">
+        <v>11112</v>
+      </c>
+      <c r="P39" s="5">
+        <v>1</v>
+      </c>
+      <c r="Q39">
+        <v>2</v>
+      </c>
+      <c r="R39" s="5">
+        <v>2.7675999999999998</v>
+      </c>
+    </row>
+    <row r="40" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A40" s="5">
+        <v>11112</v>
+      </c>
+      <c r="B40" s="5">
+        <v>2</v>
+      </c>
+      <c r="C40">
+        <v>2</v>
+      </c>
+      <c r="D40" s="5">
+        <v>2.0830000000000002</v>
+      </c>
+      <c r="O40" s="5">
+        <v>11112</v>
+      </c>
+      <c r="P40" s="5">
+        <v>2</v>
+      </c>
+      <c r="Q40">
+        <v>2</v>
+      </c>
+      <c r="R40" s="5">
+        <v>2.2237</v>
+      </c>
+    </row>
+    <row r="41" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A41" s="5">
+        <v>11112</v>
+      </c>
+      <c r="B41" s="5">
+        <v>3</v>
+      </c>
+      <c r="C41">
+        <v>2</v>
+      </c>
+      <c r="D41" s="5">
+        <v>2.3456999999999999</v>
+      </c>
+      <c r="O41" s="5">
+        <v>11112</v>
+      </c>
+      <c r="P41" s="5">
+        <v>3</v>
+      </c>
+      <c r="Q41">
+        <v>2</v>
+      </c>
+      <c r="R41" s="5">
+        <v>2.6067999999999998</v>
+      </c>
+    </row>
+    <row r="42" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A42" s="5">
+        <v>11112</v>
+      </c>
+      <c r="B42" s="5">
+        <v>4</v>
+      </c>
+      <c r="C42">
+        <v>2</v>
+      </c>
+      <c r="D42" s="5">
+        <v>2.6530999999999998</v>
+      </c>
+      <c r="O42" s="5">
+        <v>11112</v>
+      </c>
+      <c r="P42" s="5">
+        <v>4</v>
+      </c>
+      <c r="Q42">
+        <v>2</v>
+      </c>
+      <c r="R42" s="5">
+        <v>3.1389999999999998</v>
+      </c>
+    </row>
+    <row r="43" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A43" s="5">
+        <v>11112</v>
+      </c>
+      <c r="B43" s="5">
+        <v>5</v>
+      </c>
+      <c r="C43">
+        <v>2</v>
+      </c>
+      <c r="D43" s="5">
+        <v>2.9794999999999998</v>
+      </c>
+      <c r="O43" s="5">
+        <v>11112</v>
+      </c>
+      <c r="P43" s="5">
+        <v>5</v>
+      </c>
+      <c r="Q43">
+        <v>2</v>
+      </c>
+      <c r="R43" s="5">
         <v>2.4180999999999999</v>
       </c>
     </row>
@@ -3048,5 +3574,6 @@
     <mergeCell ref="Q2:R2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>